<commit_message>
Ajustado descrição do projeto
</commit_message>
<xml_diff>
--- a/Dados/Config.xlsx
+++ b/Dados/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newuser\OneDrive - xdp3s\Documentos\UiPath\Desafio_AuditoriaSOx\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newuser\OneDrive - xdp3s\Documentos\ProjetosGit\Desafio_AuditoriaSOx\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338AC1A2-7BC9-424E-B20E-5D52214821F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC984BB-8578-4D0C-A4A4-069C7013BE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,6 +175,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +493,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>